<commit_message>
minor bug fixed: -Pending(liquidation) -Liquidation tab highlight -CDD (Liquidation)
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_Liq_USD.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_Liq_USD.xlsx
@@ -278,7 +278,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,12 +297,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -730,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -815,9 +809,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1002,24 +993,31 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1030,26 +1028,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1432,7 +1418,7 @@
   <dimension ref="A1:AN39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1639,16 +1625,16 @@
       </c>
       <c r="T5" s="21"/>
       <c r="U5" s="22"/>
-      <c r="V5" s="119">
+      <c r="V5" s="108">
         <f ca="1">NOW()</f>
-        <v>43647.352894675925</v>
-      </c>
-      <c r="W5" s="119"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="119"/>
-      <c r="Z5" s="119"/>
-      <c r="AA5" s="119"/>
-      <c r="AB5" s="119"/>
+        <v>43705.530897337965</v>
+      </c>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
       <c r="AE5" s="6"/>
@@ -1770,25 +1756,25 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
       <c r="S8" s="6"/>
-      <c r="T8" s="103" t="s">
+      <c r="T8" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="104" t="s">
+      <c r="U8" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="V8" s="125" t="s">
+      <c r="V8" s="104" t="s">
         <v>44</v>
       </c>
       <c r="W8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="X8" s="103">
+      <c r="X8" s="102">
         <v>7</v>
       </c>
-      <c r="Y8" s="104">
+      <c r="Y8" s="103">
         <v>6</v>
       </c>
-      <c r="Z8" s="105">
+      <c r="Z8" s="104">
         <v>7</v>
       </c>
       <c r="AA8" s="33" t="s">
@@ -1834,51 +1820,51 @@
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
       <c r="O9" s="42"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="43"/>
-      <c r="AD9" s="43"/>
-      <c r="AE9" s="43"/>
-      <c r="AF9" s="43"/>
-      <c r="AG9" s="43"/>
-      <c r="AH9" s="43"/>
-      <c r="AI9" s="43"/>
-      <c r="AJ9" s="43"/>
-      <c r="AK9" s="43"/>
-      <c r="AL9" s="43"/>
-      <c r="AM9" s="43"/>
-      <c r="AN9" s="45"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="42"/>
+      <c r="X9" s="42"/>
+      <c r="Y9" s="42"/>
+      <c r="Z9" s="42"/>
+      <c r="AA9" s="42"/>
+      <c r="AB9" s="42"/>
+      <c r="AC9" s="42"/>
+      <c r="AD9" s="42"/>
+      <c r="AE9" s="42"/>
+      <c r="AF9" s="42"/>
+      <c r="AG9" s="42"/>
+      <c r="AH9" s="42"/>
+      <c r="AI9" s="42"/>
+      <c r="AJ9" s="42"/>
+      <c r="AK9" s="42"/>
+      <c r="AL9" s="42"/>
+      <c r="AM9" s="42"/>
+      <c r="AN9" s="44"/>
     </row>
     <row r="10" spans="1:40" ht="34.5" customHeight="1">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
       <c r="Q10" s="29"/>
       <c r="R10" s="29"/>
       <c r="S10" s="29"/>
@@ -1898,16 +1884,16 @@
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
-      <c r="AJ10" s="112" t="s">
+      <c r="AJ10" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="AK10" s="113"/>
-      <c r="AL10" s="113"/>
-      <c r="AM10" s="48"/>
+      <c r="AK10" s="109"/>
+      <c r="AL10" s="109"/>
+      <c r="AM10" s="47"/>
       <c r="AN10" s="39"/>
     </row>
     <row r="11" spans="1:40" ht="3" customHeight="1" thickBot="1">
-      <c r="A11" s="49"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -1942,56 +1928,56 @@
       <c r="AG11" s="6"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
-      <c r="AJ11" s="50"/>
+      <c r="AJ11" s="49"/>
       <c r="AK11" s="29"/>
       <c r="AL11" s="29"/>
       <c r="AM11" s="6"/>
       <c r="AN11" s="39"/>
     </row>
     <row r="12" spans="1:40" ht="3.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="53"/>
-      <c r="X12" s="53"/>
-      <c r="Y12" s="53"/>
-      <c r="Z12" s="53"/>
-      <c r="AA12" s="54"/>
-      <c r="AB12" s="54"/>
-      <c r="AC12" s="54"/>
-      <c r="AD12" s="54"/>
-      <c r="AE12" s="53"/>
-      <c r="AF12" s="54"/>
-      <c r="AG12" s="54"/>
-      <c r="AH12" s="54"/>
-      <c r="AI12" s="54"/>
-      <c r="AJ12" s="55"/>
-      <c r="AK12" s="53"/>
-      <c r="AL12" s="53"/>
-      <c r="AM12" s="54"/>
-      <c r="AN12" s="56"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="52"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
+      <c r="Y12" s="52"/>
+      <c r="Z12" s="52"/>
+      <c r="AA12" s="53"/>
+      <c r="AB12" s="53"/>
+      <c r="AC12" s="53"/>
+      <c r="AD12" s="53"/>
+      <c r="AE12" s="52"/>
+      <c r="AF12" s="53"/>
+      <c r="AG12" s="53"/>
+      <c r="AH12" s="53"/>
+      <c r="AI12" s="53"/>
+      <c r="AJ12" s="54"/>
+      <c r="AK12" s="52"/>
+      <c r="AL12" s="52"/>
+      <c r="AM12" s="53"/>
+      <c r="AN12" s="55"/>
     </row>
     <row r="13" spans="1:40" ht="3" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="57"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -2039,79 +2025,79 @@
       <c r="AN13" s="39"/>
     </row>
     <row r="14" spans="1:40" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="122" t="s">
+      <c r="B14" s="110"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="123"/>
+      <c r="F14" s="113"/>
       <c r="G14" s="29"/>
       <c r="I14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="58" t="s">
+      <c r="M14" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="59" t="s">
+      <c r="N14" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="O14" s="59" t="s">
+      <c r="O14" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="60"/>
+      <c r="P14" s="59"/>
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
       <c r="S14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="X14" s="106"/>
-      <c r="Y14" s="106"/>
-      <c r="Z14" s="106"/>
-      <c r="AA14" s="106"/>
-      <c r="AB14" s="106"/>
-      <c r="AC14" s="106"/>
-      <c r="AD14" s="106"/>
-      <c r="AE14" s="107"/>
-      <c r="AF14" s="107"/>
-      <c r="AG14" s="107"/>
-      <c r="AH14" s="107"/>
-      <c r="AI14" s="107"/>
-      <c r="AJ14" s="107"/>
-      <c r="AK14" s="108"/>
-      <c r="AL14" s="108"/>
-      <c r="AM14" s="109"/>
+      <c r="X14" s="120"/>
+      <c r="Y14" s="105"/>
+      <c r="Z14" s="105"/>
+      <c r="AA14" s="105"/>
+      <c r="AB14" s="105"/>
+      <c r="AC14" s="105"/>
+      <c r="AD14" s="105"/>
+      <c r="AE14" s="105"/>
+      <c r="AF14" s="105"/>
+      <c r="AG14" s="105"/>
+      <c r="AH14" s="105"/>
+      <c r="AI14" s="105"/>
+      <c r="AJ14" s="105"/>
+      <c r="AK14" s="105"/>
+      <c r="AL14" s="105"/>
+      <c r="AM14" s="121"/>
       <c r="AN14" s="10"/>
     </row>
     <row r="15" spans="1:40" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A15" s="111" t="s">
+      <c r="A15" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="112"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="64" t="s">
+      <c r="B15" s="107"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="65" t="s">
+      <c r="G15" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="66"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="68"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="67"/>
       <c r="R15" s="29"/>
       <c r="S15" s="29"/>
       <c r="T15" s="29"/>
@@ -2137,25 +2123,25 @@
       <c r="AN15" s="10"/>
     </row>
     <row r="16" spans="1:40" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A16" s="111" t="s">
+      <c r="A16" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="112"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="69">
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="68">
         <v>0</v>
       </c>
-      <c r="F16" s="70">
+      <c r="F16" s="69">
         <v>0</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="69">
         <v>2</v>
       </c>
-      <c r="H16" s="70">
+      <c r="H16" s="69">
         <v>0</v>
       </c>
-      <c r="I16" s="71">
+      <c r="I16" s="70">
         <v>4</v>
       </c>
       <c r="J16" s="29"/>
@@ -2170,67 +2156,67 @@
         <v>24</v>
       </c>
       <c r="W16" s="29"/>
-      <c r="Z16" s="103" t="s">
+      <c r="Z16" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="AA16" s="104">
+      <c r="AA16" s="103">
         <v>7</v>
       </c>
-      <c r="AB16" s="105">
+      <c r="AB16" s="104">
         <v>9</v>
       </c>
-      <c r="AC16" s="72" t="s">
+      <c r="AC16" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="AD16" s="103">
+      <c r="AD16" s="102">
         <v>7</v>
       </c>
-      <c r="AE16" s="104">
+      <c r="AE16" s="103">
         <v>8</v>
       </c>
-      <c r="AF16" s="105">
+      <c r="AF16" s="104">
         <v>9</v>
       </c>
-      <c r="AG16" s="72" t="s">
+      <c r="AG16" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="AH16" s="103">
+      <c r="AH16" s="102">
         <v>1</v>
       </c>
-      <c r="AI16" s="104">
+      <c r="AI16" s="103">
         <v>5</v>
       </c>
-      <c r="AJ16" s="104">
+      <c r="AJ16" s="103">
         <v>1</v>
       </c>
-      <c r="AK16" s="104">
+      <c r="AK16" s="103">
         <v>1</v>
       </c>
-      <c r="AL16" s="104">
+      <c r="AL16" s="103">
         <v>3</v>
       </c>
-      <c r="AM16" s="105">
+      <c r="AM16" s="104">
         <v>7</v>
       </c>
       <c r="AN16" s="10"/>
     </row>
     <row r="17" spans="1:40" ht="38.25" customHeight="1">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
@@ -2240,10 +2226,10 @@
       <c r="W17" s="29"/>
       <c r="X17" s="29"/>
       <c r="Y17" s="29"/>
-      <c r="Z17" s="73"/>
-      <c r="AA17" s="73"/>
-      <c r="AB17" s="73"/>
-      <c r="AC17" s="47"/>
+      <c r="Z17" s="72"/>
+      <c r="AA17" s="72"/>
+      <c r="AB17" s="72"/>
+      <c r="AC17" s="46"/>
       <c r="AF17" s="29"/>
       <c r="AG17" s="29"/>
       <c r="AH17" s="29"/>
@@ -2255,41 +2241,41 @@
       <c r="AN17" s="10"/>
     </row>
     <row r="18" spans="1:40" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
-      <c r="E18" s="47"/>
-      <c r="H18" s="124" t="s">
+      <c r="E18" s="46"/>
+      <c r="H18" s="114" t="s">
         <v>28</v>
       </c>
       <c r="I18" s="115"/>
       <c r="J18" s="115"/>
       <c r="K18" s="116"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="47"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="47"/>
-      <c r="U18" s="47"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="46"/>
       <c r="X18" s="29"/>
       <c r="Y18" s="29"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="AH18" s="47"/>
-      <c r="AI18" s="47"/>
-      <c r="AJ18" s="47"/>
-      <c r="AK18" s="47"/>
-      <c r="AL18" s="47"/>
-      <c r="AM18" s="47"/>
+      <c r="AH18" s="46"/>
+      <c r="AI18" s="46"/>
+      <c r="AJ18" s="46"/>
+      <c r="AK18" s="46"/>
+      <c r="AL18" s="46"/>
+      <c r="AM18" s="46"/>
       <c r="AN18" s="10"/>
     </row>
     <row r="19" spans="1:40" ht="39" customHeight="1" thickBot="1">
@@ -2299,54 +2285,54 @@
       <c r="B19" s="118"/>
       <c r="C19" s="118"/>
       <c r="D19" s="118"/>
-      <c r="E19" s="74"/>
+      <c r="E19" s="73"/>
       <c r="F19" s="29" t="s">
         <v>31</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="75"/>
-      <c r="V19" s="75"/>
-      <c r="W19" s="75"/>
-      <c r="X19" s="75"/>
-      <c r="Y19" s="76"/>
-      <c r="Z19" s="75"/>
-      <c r="AA19" s="75"/>
-      <c r="AB19" s="75"/>
-      <c r="AC19" s="75"/>
-      <c r="AD19" s="75"/>
-      <c r="AE19" s="75"/>
-      <c r="AF19" s="75"/>
-      <c r="AG19" s="75"/>
-      <c r="AH19" s="75"/>
-      <c r="AI19" s="75"/>
-      <c r="AJ19" s="75"/>
-      <c r="AK19" s="75"/>
-      <c r="AL19" s="75"/>
-      <c r="AM19" s="75"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="74"/>
+      <c r="S19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="74"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="74"/>
+      <c r="X19" s="74"/>
+      <c r="Y19" s="75"/>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="74"/>
+      <c r="AB19" s="74"/>
+      <c r="AC19" s="74"/>
+      <c r="AD19" s="74"/>
+      <c r="AE19" s="74"/>
+      <c r="AF19" s="74"/>
+      <c r="AG19" s="74"/>
+      <c r="AH19" s="74"/>
+      <c r="AI19" s="74"/>
+      <c r="AJ19" s="74"/>
+      <c r="AK19" s="74"/>
+      <c r="AL19" s="74"/>
+      <c r="AM19" s="74"/>
       <c r="AN19" s="10"/>
     </row>
     <row r="20" spans="1:40" ht="36" customHeight="1" thickBot="1">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
       <c r="E20" s="34">
         <v>0</v>
       </c>
-      <c r="F20" s="61">
+      <c r="F20" s="60">
         <v>1</v>
       </c>
       <c r="G20" s="32">
@@ -2371,41 +2357,41 @@
       <c r="U20" s="29"/>
       <c r="V20" s="29"/>
       <c r="W20" s="29"/>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="47"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="47"/>
-      <c r="AC20" s="47"/>
-      <c r="AD20" s="47"/>
-      <c r="AE20" s="47"/>
-      <c r="AF20" s="47"/>
-      <c r="AG20" s="47"/>
-      <c r="AH20" s="47"/>
-      <c r="AI20" s="47"/>
-      <c r="AJ20" s="48"/>
-      <c r="AK20" s="47"/>
-      <c r="AL20" s="47"/>
-      <c r="AM20" s="47"/>
+      <c r="X20" s="46"/>
+      <c r="Y20" s="46"/>
+      <c r="Z20" s="46"/>
+      <c r="AA20" s="46"/>
+      <c r="AB20" s="46"/>
+      <c r="AC20" s="46"/>
+      <c r="AD20" s="46"/>
+      <c r="AE20" s="46"/>
+      <c r="AF20" s="46"/>
+      <c r="AG20" s="46"/>
+      <c r="AH20" s="46"/>
+      <c r="AI20" s="46"/>
+      <c r="AJ20" s="47"/>
+      <c r="AK20" s="46"/>
+      <c r="AL20" s="46"/>
+      <c r="AM20" s="46"/>
       <c r="AN20" s="39"/>
     </row>
     <row r="21" spans="1:40" ht="36" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -2434,7 +2420,7 @@
       <c r="AN21" s="39"/>
     </row>
     <row r="22" spans="1:40" ht="3" customHeight="1" thickBot="1">
-      <c r="A22" s="46"/>
+      <c r="A22" s="45"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
@@ -2476,49 +2462,49 @@
       <c r="AN22" s="39"/>
     </row>
     <row r="23" spans="1:40" ht="3.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A23" s="78"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="53"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="53"/>
-      <c r="V23" s="53"/>
-      <c r="W23" s="53"/>
-      <c r="X23" s="53"/>
-      <c r="Y23" s="53"/>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="53"/>
-      <c r="AC23" s="53"/>
-      <c r="AD23" s="53"/>
-      <c r="AE23" s="53"/>
-      <c r="AF23" s="53"/>
-      <c r="AG23" s="53"/>
-      <c r="AH23" s="53"/>
-      <c r="AI23" s="53"/>
-      <c r="AJ23" s="53"/>
-      <c r="AK23" s="53"/>
-      <c r="AL23" s="53"/>
-      <c r="AM23" s="53"/>
-      <c r="AN23" s="56"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="52"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="52"/>
+      <c r="AA23" s="52"/>
+      <c r="AB23" s="52"/>
+      <c r="AC23" s="52"/>
+      <c r="AD23" s="52"/>
+      <c r="AE23" s="52"/>
+      <c r="AF23" s="52"/>
+      <c r="AG23" s="52"/>
+      <c r="AH23" s="52"/>
+      <c r="AI23" s="52"/>
+      <c r="AJ23" s="52"/>
+      <c r="AK23" s="52"/>
+      <c r="AL23" s="52"/>
+      <c r="AM23" s="52"/>
+      <c r="AN23" s="55"/>
     </row>
     <row r="24" spans="1:40" s="12" customFormat="1" ht="3" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A24" s="79"/>
+      <c r="A24" s="78"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
@@ -2560,84 +2546,84 @@
       <c r="AN24" s="39"/>
     </row>
     <row r="25" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A25" s="111" t="s">
+      <c r="A25" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="121"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="122" t="s">
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="123"/>
+      <c r="F25" s="113"/>
       <c r="G25" s="29"/>
       <c r="I25" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="M25" s="58" t="s">
+      <c r="M25" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="59" t="s">
+      <c r="N25" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="O25" s="59" t="s">
+      <c r="O25" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="P25" s="60"/>
+      <c r="P25" s="59"/>
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
       <c r="S25" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="T25" s="68"/>
-      <c r="U25" s="68"/>
-      <c r="V25" s="68"/>
-      <c r="W25" s="80"/>
-      <c r="X25" s="106"/>
-      <c r="Y25" s="106"/>
-      <c r="Z25" s="106"/>
-      <c r="AA25" s="106"/>
-      <c r="AB25" s="106"/>
-      <c r="AC25" s="106"/>
-      <c r="AD25" s="106"/>
-      <c r="AE25" s="107"/>
-      <c r="AF25" s="108"/>
-      <c r="AG25" s="108"/>
-      <c r="AH25" s="108"/>
-      <c r="AI25" s="108"/>
-      <c r="AJ25" s="108"/>
-      <c r="AK25" s="108"/>
-      <c r="AL25" s="108"/>
-      <c r="AM25" s="110"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="67"/>
+      <c r="V25" s="67"/>
+      <c r="W25" s="79"/>
+      <c r="X25" s="120"/>
+      <c r="Y25" s="105"/>
+      <c r="Z25" s="105"/>
+      <c r="AA25" s="105"/>
+      <c r="AB25" s="105"/>
+      <c r="AC25" s="105"/>
+      <c r="AD25" s="105"/>
+      <c r="AE25" s="105"/>
+      <c r="AF25" s="105"/>
+      <c r="AG25" s="105"/>
+      <c r="AH25" s="105"/>
+      <c r="AI25" s="105"/>
+      <c r="AJ25" s="105"/>
+      <c r="AK25" s="105"/>
+      <c r="AL25" s="105"/>
+      <c r="AM25" s="121"/>
       <c r="AN25" s="10"/>
     </row>
     <row r="26" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="112"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112"/>
+      <c r="B26" s="107"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="107"/>
       <c r="E26" s="34">
         <v>9</v>
       </c>
-      <c r="F26" s="61">
+      <c r="F26" s="60">
         <v>0</v>
       </c>
-      <c r="G26" s="61">
+      <c r="G26" s="60">
         <v>0</v>
       </c>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="62"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="68"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="67"/>
       <c r="S26" s="29"/>
       <c r="T26" s="29"/>
       <c r="U26" s="29"/>
@@ -2662,25 +2648,25 @@
       <c r="AN26" s="10"/>
     </row>
     <row r="27" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="112"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="69">
+      <c r="B27" s="107"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="68">
         <v>1</v>
       </c>
-      <c r="F27" s="70">
+      <c r="F27" s="69">
         <v>4</v>
       </c>
-      <c r="G27" s="70">
+      <c r="G27" s="69">
         <v>0</v>
       </c>
-      <c r="H27" s="70">
+      <c r="H27" s="69">
         <v>1</v>
       </c>
-      <c r="I27" s="71">
+      <c r="I27" s="70">
         <v>7</v>
       </c>
       <c r="J27" s="29"/>
@@ -2700,67 +2686,67 @@
       <c r="W27" s="29"/>
       <c r="X27" s="29"/>
       <c r="Y27" s="29"/>
-      <c r="Z27" s="103" t="s">
+      <c r="Z27" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="AA27" s="104">
+      <c r="AA27" s="103">
         <v>7</v>
       </c>
-      <c r="AB27" s="105">
+      <c r="AB27" s="104">
         <v>9</v>
       </c>
-      <c r="AC27" s="72" t="s">
+      <c r="AC27" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="AD27" s="103">
+      <c r="AD27" s="102">
         <v>7</v>
       </c>
-      <c r="AE27" s="104">
+      <c r="AE27" s="103">
         <v>8</v>
       </c>
-      <c r="AF27" s="105">
+      <c r="AF27" s="104">
         <v>9</v>
       </c>
-      <c r="AG27" s="72" t="s">
+      <c r="AG27" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="AH27" s="103">
+      <c r="AH27" s="102">
         <v>1</v>
       </c>
-      <c r="AI27" s="104">
+      <c r="AI27" s="103">
         <v>1</v>
       </c>
-      <c r="AJ27" s="104">
+      <c r="AJ27" s="103">
         <v>1</v>
       </c>
-      <c r="AK27" s="104">
+      <c r="AK27" s="103">
         <v>1</v>
       </c>
-      <c r="AL27" s="104">
+      <c r="AL27" s="103">
         <v>1</v>
       </c>
-      <c r="AM27" s="105">
+      <c r="AM27" s="104">
         <v>1</v>
       </c>
       <c r="AN27" s="10"/>
     </row>
     <row r="28" spans="1:40" s="12" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A28" s="111" t="s">
+      <c r="A28" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
+      <c r="B28" s="109"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
@@ -2773,10 +2759,10 @@
       <c r="W28" s="29"/>
       <c r="X28" s="29"/>
       <c r="Y28" s="29"/>
-      <c r="Z28" s="73"/>
-      <c r="AA28" s="73"/>
-      <c r="AB28" s="73"/>
-      <c r="AC28" s="47"/>
+      <c r="Z28" s="72"/>
+      <c r="AA28" s="72"/>
+      <c r="AB28" s="72"/>
+      <c r="AC28" s="46"/>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="29"/>
@@ -2790,29 +2776,29 @@
       <c r="AN28" s="10"/>
     </row>
     <row r="29" spans="1:40" s="12" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="45" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
-      <c r="E29" s="47"/>
-      <c r="H29" s="114" t="s">
+      <c r="E29" s="46"/>
+      <c r="H29" s="119" t="s">
         <v>28</v>
       </c>
       <c r="I29" s="115"/>
       <c r="J29" s="115"/>
       <c r="K29" s="116"/>
-      <c r="L29" s="82"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
-      <c r="Q29" s="47"/>
-      <c r="R29" s="47"/>
-      <c r="S29" s="47"/>
-      <c r="T29" s="47"/>
-      <c r="U29" s="47"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="46"/>
       <c r="W29" s="4"/>
       <c r="X29" s="29"/>
       <c r="Y29" s="29"/>
@@ -2820,12 +2806,12 @@
       <c r="AB29" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="AH29" s="47"/>
-      <c r="AI29" s="47"/>
-      <c r="AJ29" s="47"/>
-      <c r="AK29" s="47"/>
-      <c r="AL29" s="47"/>
-      <c r="AM29" s="47"/>
+      <c r="AH29" s="46"/>
+      <c r="AI29" s="46"/>
+      <c r="AJ29" s="46"/>
+      <c r="AK29" s="46"/>
+      <c r="AL29" s="46"/>
+      <c r="AM29" s="46"/>
       <c r="AN29" s="10"/>
     </row>
     <row r="30" spans="1:40" s="12" customFormat="1" ht="39" customHeight="1" thickBot="1">
@@ -2835,55 +2821,55 @@
       <c r="B30" s="118"/>
       <c r="C30" s="118"/>
       <c r="D30" s="118"/>
-      <c r="E30" s="74"/>
+      <c r="E30" s="73"/>
       <c r="F30" s="29" t="s">
         <v>31</v>
       </c>
       <c r="H30" s="29"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="47"/>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="47"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="47"/>
-      <c r="Y30" s="47"/>
-      <c r="Z30" s="47"/>
-      <c r="AA30" s="47"/>
-      <c r="AB30" s="47"/>
-      <c r="AC30" s="47"/>
-      <c r="AD30" s="47"/>
-      <c r="AE30" s="47"/>
-      <c r="AF30" s="47"/>
-      <c r="AG30" s="47"/>
-      <c r="AH30" s="47"/>
-      <c r="AI30" s="47"/>
-      <c r="AJ30" s="47"/>
-      <c r="AK30" s="47"/>
-      <c r="AL30" s="47"/>
-      <c r="AM30" s="47"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="46"/>
+      <c r="V30" s="46"/>
+      <c r="W30" s="46"/>
+      <c r="X30" s="46"/>
+      <c r="Y30" s="46"/>
+      <c r="Z30" s="46"/>
+      <c r="AA30" s="46"/>
+      <c r="AB30" s="46"/>
+      <c r="AC30" s="46"/>
+      <c r="AD30" s="46"/>
+      <c r="AE30" s="46"/>
+      <c r="AF30" s="46"/>
+      <c r="AG30" s="46"/>
+      <c r="AH30" s="46"/>
+      <c r="AI30" s="46"/>
+      <c r="AJ30" s="46"/>
+      <c r="AK30" s="46"/>
+      <c r="AL30" s="46"/>
+      <c r="AM30" s="46"/>
       <c r="AN30" s="10"/>
     </row>
     <row r="31" spans="1:40" s="12" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
       <c r="E31" s="34">
         <v>0</v>
       </c>
-      <c r="F31" s="61">
+      <c r="F31" s="60">
         <v>1</v>
       </c>
       <c r="G31" s="32">
@@ -2910,41 +2896,41 @@
       <c r="U31" s="29"/>
       <c r="V31" s="29"/>
       <c r="W31" s="29"/>
-      <c r="X31" s="47"/>
-      <c r="Y31" s="47"/>
-      <c r="Z31" s="47"/>
-      <c r="AA31" s="47"/>
-      <c r="AB31" s="47"/>
-      <c r="AC31" s="47"/>
-      <c r="AD31" s="47"/>
-      <c r="AE31" s="47"/>
-      <c r="AF31" s="47"/>
-      <c r="AG31" s="47"/>
-      <c r="AH31" s="47"/>
-      <c r="AI31" s="47"/>
-      <c r="AJ31" s="48"/>
-      <c r="AK31" s="47"/>
-      <c r="AL31" s="47"/>
-      <c r="AM31" s="47"/>
+      <c r="X31" s="46"/>
+      <c r="Y31" s="46"/>
+      <c r="Z31" s="46"/>
+      <c r="AA31" s="46"/>
+      <c r="AB31" s="46"/>
+      <c r="AC31" s="46"/>
+      <c r="AD31" s="46"/>
+      <c r="AE31" s="46"/>
+      <c r="AF31" s="46"/>
+      <c r="AG31" s="46"/>
+      <c r="AH31" s="46"/>
+      <c r="AI31" s="46"/>
+      <c r="AJ31" s="47"/>
+      <c r="AK31" s="46"/>
+      <c r="AL31" s="46"/>
+      <c r="AM31" s="46"/>
       <c r="AN31" s="39"/>
     </row>
     <row r="32" spans="1:40" s="12" customFormat="1" ht="36" customHeight="1">
-      <c r="A32" s="111" t="s">
+      <c r="A32" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="112"/>
-      <c r="C32" s="112"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
+      <c r="B32" s="107"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
@@ -2973,230 +2959,230 @@
       <c r="AN32" s="39"/>
     </row>
     <row r="33" spans="1:40" s="12" customFormat="1" ht="5.25" customHeight="1" thickBot="1">
-      <c r="A33" s="83"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="84"/>
-      <c r="J33" s="84"/>
-      <c r="K33" s="84"/>
-      <c r="L33" s="84"/>
-      <c r="M33" s="84"/>
-      <c r="N33" s="84"/>
-      <c r="O33" s="84"/>
-      <c r="P33" s="84"/>
-      <c r="Q33" s="84"/>
-      <c r="R33" s="84"/>
-      <c r="S33" s="84"/>
-      <c r="T33" s="84"/>
-      <c r="U33" s="84"/>
-      <c r="V33" s="84"/>
-      <c r="W33" s="84"/>
-      <c r="X33" s="84"/>
-      <c r="Y33" s="84"/>
-      <c r="Z33" s="84"/>
-      <c r="AA33" s="84"/>
-      <c r="AB33" s="84"/>
-      <c r="AC33" s="84"/>
-      <c r="AD33" s="84"/>
-      <c r="AE33" s="84"/>
-      <c r="AF33" s="84"/>
-      <c r="AG33" s="84"/>
-      <c r="AH33" s="84"/>
-      <c r="AI33" s="84"/>
-      <c r="AJ33" s="84"/>
-      <c r="AK33" s="84"/>
-      <c r="AL33" s="84"/>
-      <c r="AM33" s="84"/>
-      <c r="AN33" s="85"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="83"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="83"/>
+      <c r="Q33" s="83"/>
+      <c r="R33" s="83"/>
+      <c r="S33" s="83"/>
+      <c r="T33" s="83"/>
+      <c r="U33" s="83"/>
+      <c r="V33" s="83"/>
+      <c r="W33" s="83"/>
+      <c r="X33" s="83"/>
+      <c r="Y33" s="83"/>
+      <c r="Z33" s="83"/>
+      <c r="AA33" s="83"/>
+      <c r="AB33" s="83"/>
+      <c r="AC33" s="83"/>
+      <c r="AD33" s="83"/>
+      <c r="AE33" s="83"/>
+      <c r="AF33" s="83"/>
+      <c r="AG33" s="83"/>
+      <c r="AH33" s="83"/>
+      <c r="AI33" s="83"/>
+      <c r="AJ33" s="83"/>
+      <c r="AK33" s="83"/>
+      <c r="AL33" s="83"/>
+      <c r="AM33" s="83"/>
+      <c r="AN33" s="84"/>
     </row>
     <row r="34" spans="1:40" s="12" customFormat="1" ht="6" customHeight="1" thickTop="1">
-      <c r="A34" s="68"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="68"/>
-      <c r="R34" s="68"/>
-      <c r="S34" s="68"/>
-      <c r="T34" s="68"/>
-      <c r="U34" s="68"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="67"/>
+      <c r="T34" s="67"/>
+      <c r="U34" s="67"/>
     </row>
     <row r="35" spans="1:40" ht="16.5" customHeight="1">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-      <c r="M35" s="86"/>
-      <c r="N35" s="86"/>
-      <c r="O35" s="86"/>
-      <c r="P35" s="87" t="s">
+      <c r="A35" s="85"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="85"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="85"/>
+      <c r="P35" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="88"/>
-      <c r="S35" s="88"/>
-      <c r="T35" s="88"/>
-      <c r="U35" s="89"/>
-      <c r="V35" s="89"/>
-      <c r="W35" s="89"/>
-      <c r="X35" s="90"/>
-      <c r="Y35" s="88" t="s">
+      <c r="Q35" s="87"/>
+      <c r="R35" s="87"/>
+      <c r="S35" s="87"/>
+      <c r="T35" s="87"/>
+      <c r="U35" s="88"/>
+      <c r="V35" s="88"/>
+      <c r="W35" s="88"/>
+      <c r="X35" s="89"/>
+      <c r="Y35" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="Z35" s="88"/>
-      <c r="AA35" s="89"/>
-      <c r="AB35" s="88"/>
-      <c r="AC35" s="90"/>
-      <c r="AD35" s="88" t="s">
+      <c r="Z35" s="87"/>
+      <c r="AA35" s="88"/>
+      <c r="AB35" s="87"/>
+      <c r="AC35" s="89"/>
+      <c r="AD35" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="AE35" s="88"/>
-      <c r="AF35" s="89"/>
-      <c r="AG35" s="88"/>
-      <c r="AH35" s="90"/>
-      <c r="AI35" s="87" t="s">
+      <c r="AE35" s="87"/>
+      <c r="AF35" s="88"/>
+      <c r="AG35" s="87"/>
+      <c r="AH35" s="89"/>
+      <c r="AI35" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="AJ35" s="88"/>
-      <c r="AK35" s="88"/>
-      <c r="AL35" s="88"/>
-      <c r="AM35" s="90"/>
+      <c r="AJ35" s="87"/>
+      <c r="AK35" s="87"/>
+      <c r="AL35" s="87"/>
+      <c r="AM35" s="89"/>
     </row>
     <row r="36" spans="1:40" ht="15.75" customHeight="1">
-      <c r="A36" s="86"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-      <c r="M36" s="86"/>
-      <c r="N36" s="86"/>
-      <c r="O36" s="86"/>
-      <c r="P36" s="91"/>
-      <c r="Q36" s="92"/>
-      <c r="R36" s="92"/>
-      <c r="S36" s="92"/>
-      <c r="T36" s="92"/>
+      <c r="A36" s="85"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="85"/>
+      <c r="K36" s="85"/>
+      <c r="L36" s="85"/>
+      <c r="M36" s="85"/>
+      <c r="N36" s="85"/>
+      <c r="O36" s="85"/>
+      <c r="P36" s="90"/>
+      <c r="Q36" s="91"/>
+      <c r="R36" s="91"/>
+      <c r="S36" s="91"/>
+      <c r="T36" s="91"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="6"/>
-      <c r="X36" s="93"/>
-      <c r="Y36" s="94"/>
-      <c r="Z36" s="95"/>
-      <c r="AA36" s="95"/>
-      <c r="AB36" s="95"/>
-      <c r="AC36" s="96"/>
-      <c r="AD36" s="94"/>
-      <c r="AE36" s="95"/>
-      <c r="AF36" s="95"/>
-      <c r="AG36" s="95"/>
-      <c r="AH36" s="96"/>
-      <c r="AI36" s="94"/>
-      <c r="AJ36" s="95"/>
-      <c r="AK36" s="95"/>
-      <c r="AL36" s="95"/>
-      <c r="AM36" s="96"/>
+      <c r="X36" s="92"/>
+      <c r="Y36" s="93"/>
+      <c r="Z36" s="94"/>
+      <c r="AA36" s="94"/>
+      <c r="AB36" s="94"/>
+      <c r="AC36" s="95"/>
+      <c r="AD36" s="93"/>
+      <c r="AE36" s="94"/>
+      <c r="AF36" s="94"/>
+      <c r="AG36" s="94"/>
+      <c r="AH36" s="95"/>
+      <c r="AI36" s="93"/>
+      <c r="AJ36" s="94"/>
+      <c r="AK36" s="94"/>
+      <c r="AL36" s="94"/>
+      <c r="AM36" s="95"/>
     </row>
     <row r="37" spans="1:40" ht="15.75" customHeight="1">
-      <c r="A37" s="86"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
-      <c r="M37" s="86"/>
-      <c r="N37" s="86"/>
-      <c r="O37" s="86"/>
-      <c r="P37" s="91"/>
-      <c r="Q37" s="92"/>
-      <c r="R37" s="92"/>
-      <c r="S37" s="92"/>
-      <c r="T37" s="92"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="85"/>
+      <c r="O37" s="85"/>
+      <c r="P37" s="90"/>
+      <c r="Q37" s="91"/>
+      <c r="R37" s="91"/>
+      <c r="S37" s="91"/>
+      <c r="T37" s="91"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
       <c r="W37" s="6"/>
-      <c r="X37" s="93"/>
-      <c r="Y37" s="94"/>
-      <c r="Z37" s="95"/>
-      <c r="AA37" s="95"/>
-      <c r="AB37" s="95"/>
-      <c r="AC37" s="96"/>
-      <c r="AD37" s="94"/>
-      <c r="AE37" s="95"/>
-      <c r="AF37" s="95"/>
-      <c r="AG37" s="95"/>
-      <c r="AH37" s="96"/>
-      <c r="AI37" s="94"/>
-      <c r="AJ37" s="95"/>
-      <c r="AK37" s="95"/>
-      <c r="AL37" s="95"/>
-      <c r="AM37" s="96"/>
+      <c r="X37" s="92"/>
+      <c r="Y37" s="93"/>
+      <c r="Z37" s="94"/>
+      <c r="AA37" s="94"/>
+      <c r="AB37" s="94"/>
+      <c r="AC37" s="95"/>
+      <c r="AD37" s="93"/>
+      <c r="AE37" s="94"/>
+      <c r="AF37" s="94"/>
+      <c r="AG37" s="94"/>
+      <c r="AH37" s="95"/>
+      <c r="AI37" s="93"/>
+      <c r="AJ37" s="94"/>
+      <c r="AK37" s="94"/>
+      <c r="AL37" s="94"/>
+      <c r="AM37" s="95"/>
     </row>
     <row r="38" spans="1:40" ht="15.75" customHeight="1">
-      <c r="A38" s="86"/>
-      <c r="P38" s="97"/>
-      <c r="Q38" s="98"/>
-      <c r="R38" s="98"/>
-      <c r="S38" s="98"/>
-      <c r="T38" s="98"/>
+      <c r="A38" s="85"/>
+      <c r="P38" s="96"/>
+      <c r="Q38" s="97"/>
+      <c r="R38" s="97"/>
+      <c r="S38" s="97"/>
+      <c r="T38" s="97"/>
       <c r="U38" s="24"/>
       <c r="V38" s="24"/>
       <c r="W38" s="24"/>
-      <c r="X38" s="99"/>
-      <c r="Y38" s="100"/>
-      <c r="Z38" s="101"/>
-      <c r="AA38" s="101"/>
-      <c r="AB38" s="101"/>
-      <c r="AC38" s="102"/>
-      <c r="AD38" s="100"/>
-      <c r="AE38" s="101"/>
-      <c r="AF38" s="101"/>
-      <c r="AG38" s="101"/>
-      <c r="AH38" s="102"/>
-      <c r="AI38" s="100"/>
-      <c r="AJ38" s="101"/>
-      <c r="AK38" s="101"/>
-      <c r="AL38" s="101"/>
-      <c r="AM38" s="102"/>
+      <c r="X38" s="98"/>
+      <c r="Y38" s="99"/>
+      <c r="Z38" s="100"/>
+      <c r="AA38" s="100"/>
+      <c r="AB38" s="100"/>
+      <c r="AC38" s="101"/>
+      <c r="AD38" s="99"/>
+      <c r="AE38" s="100"/>
+      <c r="AF38" s="100"/>
+      <c r="AG38" s="100"/>
+      <c r="AH38" s="101"/>
+      <c r="AI38" s="99"/>
+      <c r="AJ38" s="100"/>
+      <c r="AK38" s="100"/>
+      <c r="AL38" s="100"/>
+      <c r="AM38" s="101"/>
     </row>
     <row r="39" spans="1:40">
-      <c r="A39" s="86"/>
+      <c r="A39" s="85"/>
       <c r="V39" s="6"/>
       <c r="W39" s="29"/>
       <c r="X39" s="29"/>
@@ -3219,6 +3205,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A32:D32"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="V5:AB5"/>
     <mergeCell ref="AJ10:AL10"/>
@@ -3231,11 +3222,6 @@
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A32:D32"/>
   </mergeCells>
   <pageMargins left="0.28999999999999998" right="0.16" top="0.54" bottom="0.24" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>

</xml_diff>